<commit_message>
Adjust css for fileInput comp
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -445,8 +445,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="D4">
-        <v>21</v>
+      <c r="D4" t="str">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>